<commit_message>
Updated all notebooks to correct the model for iDK1463, published by Kim et al. (2021). The resulting tables were also updated. Added notebook 3.3 to import reactions from iDK1463 and update all reactions and genes.
</commit_message>
<xml_diff>
--- a/tables/13C_fluxes.xlsx
+++ b/tables/13C_fluxes.xlsx
@@ -24,162 +24,168 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>AKGDH</t>
   </si>
   <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>ENO</t>
+  </si>
+  <si>
+    <t>FUM</t>
+  </si>
+  <si>
+    <t>TKT2</t>
+  </si>
+  <si>
+    <t>TKT1</t>
+  </si>
+  <si>
+    <t>ICDHyr</t>
+  </si>
+  <si>
+    <t>MDH</t>
+  </si>
+  <si>
+    <t>PDH</t>
+  </si>
+  <si>
+    <t>PFK</t>
+  </si>
+  <si>
+    <t>PGI</t>
+  </si>
+  <si>
+    <t>PGK</t>
+  </si>
+  <si>
+    <t>PPC</t>
+  </si>
+  <si>
+    <t>ACKr</t>
+  </si>
+  <si>
+    <t>PYK</t>
+  </si>
+  <si>
+    <t>G6PDH2r</t>
+  </si>
+  <si>
+    <t>AKG → Suc + CO2</t>
+  </si>
+  <si>
+    <t>FBP ↔ GAP + GAP</t>
+  </si>
+  <si>
+    <t>OAA + AcCoA → Cit</t>
+  </si>
+  <si>
+    <t>6PG → GAP + Pyr</t>
+  </si>
+  <si>
+    <t>PGA ↔ PEP</t>
+  </si>
+  <si>
+    <t>Suc → Mal</t>
+  </si>
+  <si>
+    <t>6PG → R5P + CO2</t>
+  </si>
+  <si>
+    <t>R5P ↔ GAP + E2</t>
+  </si>
+  <si>
+    <t>F6P ↔ E4P + E2</t>
+  </si>
+  <si>
+    <t>R5P + E2 ↔ S7P</t>
+  </si>
+  <si>
+    <t>GAP + E3 ↔ F6P</t>
+  </si>
+  <si>
+    <t>E4P + E3 ↔ S7P</t>
+  </si>
+  <si>
+    <t>Cit → AKG + CO2</t>
+  </si>
+  <si>
+    <t>Mal ↔ OAA</t>
+  </si>
+  <si>
+    <t>Pyr → AcCoA + CO2</t>
+  </si>
+  <si>
+    <t>F6P ↔ FBP</t>
+  </si>
+  <si>
+    <t>G6P ↔ F6P</t>
+  </si>
+  <si>
+    <t>GAP ↔ PGA</t>
+  </si>
+  <si>
+    <t>PEP + CO2 ↔ OAA</t>
+  </si>
+  <si>
+    <t>Mal → Pyr + CO2</t>
+  </si>
+  <si>
+    <t>AcCoA → Acetate</t>
+  </si>
+  <si>
+    <t>PEP ↔ Pyr</t>
+  </si>
+  <si>
+    <t>G6P → 6PG</t>
+  </si>
+  <si>
+    <t>Reaction</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>ME1</t>
+  </si>
+  <si>
+    <t>ME2</t>
+  </si>
+  <si>
+    <t>RPI</t>
+  </si>
+  <si>
+    <t>glcn_flux_mean</t>
+  </si>
+  <si>
+    <t>glcn_flux_sd</t>
+  </si>
+  <si>
+    <t>Glucose + PEP → G6P + Pyr/Gluconate → 6PG</t>
+  </si>
+  <si>
+    <t>glc_flux_mean</t>
+  </si>
+  <si>
+    <t>glc_flux_sd</t>
+  </si>
+  <si>
+    <t>EDA</t>
+  </si>
+  <si>
+    <t>DMALRED</t>
+  </si>
+  <si>
+    <t>TPI</t>
+  </si>
+  <si>
     <t>FBA</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>ENO</t>
-  </si>
-  <si>
-    <t>FUM</t>
-  </si>
-  <si>
-    <t>TKT2</t>
-  </si>
-  <si>
-    <t>TKT1</t>
-  </si>
-  <si>
-    <t>ICDHyr</t>
-  </si>
-  <si>
-    <t>MDH</t>
-  </si>
-  <si>
-    <t>PDH</t>
-  </si>
-  <si>
-    <t>PFK</t>
-  </si>
-  <si>
-    <t>PGI</t>
-  </si>
-  <si>
-    <t>PGK</t>
-  </si>
-  <si>
-    <t>PPC</t>
-  </si>
-  <si>
-    <t>ACKr</t>
-  </si>
-  <si>
-    <t>PYK</t>
-  </si>
-  <si>
-    <t>G6PDH2r</t>
-  </si>
-  <si>
-    <t>AKG → Suc + CO2</t>
-  </si>
-  <si>
-    <t>FBP ↔ GAP + GAP</t>
-  </si>
-  <si>
-    <t>OAA + AcCoA → Cit</t>
-  </si>
-  <si>
-    <t>6PG → GAP + Pyr</t>
-  </si>
-  <si>
-    <t>PGA ↔ PEP</t>
-  </si>
-  <si>
-    <t>Suc → Mal</t>
-  </si>
-  <si>
-    <t>6PG → R5P + CO2</t>
-  </si>
-  <si>
-    <t>R5P ↔ GAP + E2</t>
-  </si>
-  <si>
-    <t>F6P ↔ E4P + E2</t>
-  </si>
-  <si>
-    <t>R5P + E2 ↔ S7P</t>
-  </si>
-  <si>
-    <t>GAP + E3 ↔ F6P</t>
-  </si>
-  <si>
-    <t>E4P + E3 ↔ S7P</t>
-  </si>
-  <si>
-    <t>Cit → AKG + CO2</t>
-  </si>
-  <si>
-    <t>Mal ↔ OAA</t>
-  </si>
-  <si>
-    <t>Pyr → AcCoA + CO2</t>
-  </si>
-  <si>
-    <t>F6P ↔ FBP</t>
-  </si>
-  <si>
-    <t>G6P ↔ F6P</t>
-  </si>
-  <si>
-    <t>GAP ↔ PGA</t>
-  </si>
-  <si>
-    <t>PEP + CO2 ↔ OAA</t>
-  </si>
-  <si>
-    <t>Mal → Pyr + CO2</t>
-  </si>
-  <si>
-    <t>AcCoA → Acetate</t>
-  </si>
-  <si>
-    <t>PEP ↔ Pyr</t>
-  </si>
-  <si>
-    <t>G6P → 6PG</t>
-  </si>
-  <si>
-    <t>Reaction</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>ME1</t>
-  </si>
-  <si>
-    <t>ME2</t>
-  </si>
-  <si>
-    <t>RPI</t>
-  </si>
-  <si>
-    <t>glcn_flux_mean</t>
-  </si>
-  <si>
-    <t>glcn_flux_sd</t>
-  </si>
-  <si>
-    <t>Glucose + PEP → G6P + Pyr/Gluconate → 6PG</t>
-  </si>
-  <si>
-    <t>glc_flux_mean</t>
-  </si>
-  <si>
-    <t>glc_flux_sd</t>
-  </si>
-  <si>
-    <t>EDA</t>
   </si>
 </sst>
 </file>
@@ -552,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,45 +575,45 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>41</v>
-      </c>
       <c r="C1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>50</v>
-      </c>
       <c r="E1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="7">
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -627,10 +633,10 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C4" s="3">
         <v>0.71499999999999986</v>
@@ -647,167 +653,169 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="C5" s="3">
-        <v>0.59233333333333327</v>
+        <v>0.71499999999999986</v>
       </c>
       <c r="D5" s="3">
-        <v>8.5049005481153891E-3</v>
+        <v>2.5632011235952615E-2</v>
       </c>
       <c r="E5" s="7">
-        <v>0.71133959924927037</v>
+        <v>8.8320720625593541E-2</v>
       </c>
       <c r="F5" s="7">
-        <v>6.8510243940335478E-3</v>
+        <v>6.4799155581466801E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
-        <v>0.16666666666666666</v>
+        <v>0.59233333333333327</v>
       </c>
       <c r="D6" s="3">
-        <v>3.7166292972710346E-2</v>
+        <v>8.5049005481153891E-3</v>
       </c>
       <c r="E6" s="7">
-        <v>0.8082791062242366</v>
+        <v>0.71133959924927037</v>
       </c>
       <c r="F6" s="7">
-        <v>1.1768750792201977E-2</v>
+        <v>6.8510243940335478E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3">
-        <v>1.5109999999999999</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D7" s="3">
-        <v>2.5632011235952566E-2</v>
+        <v>3.7166292972710346E-2</v>
       </c>
       <c r="E7" s="7">
-        <v>0.97138479469964401</v>
+        <v>0.8082791062242366</v>
       </c>
       <c r="F7" s="7">
-        <v>6.4799155581467521E-3</v>
+        <v>1.1768750792201977E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" s="3">
-        <v>0.52333333333333332</v>
+        <v>1.5109999999999999</v>
       </c>
       <c r="D8" s="3">
-        <v>7.5718777944003713E-3</v>
+        <v>2.5632011235952566E-2</v>
       </c>
       <c r="E8" s="7">
-        <v>0.67141737702707072</v>
+        <v>0.97138479469964401</v>
       </c>
       <c r="F8" s="7">
-        <v>6.8510243940338887E-3</v>
+        <v>6.4799155581467521E-3</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C9" s="3">
-        <v>0.17166666666666666</v>
+        <v>0.52333333333333332</v>
       </c>
       <c r="D9" s="3">
-        <v>3.2516662395352641E-2</v>
+        <v>7.5718777944003713E-3</v>
       </c>
       <c r="E9" s="7">
-        <v>0.19780127335509068</v>
+        <v>0.67141737702707072</v>
       </c>
       <c r="F9" s="7">
-        <v>1.9392284348197522E-2</v>
+        <v>6.8510243940338887E-3</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C10" s="3">
-        <v>6.7666666666666667E-2</v>
+        <v>0.17166666666666666</v>
       </c>
       <c r="D10" s="3">
-        <v>2.1939310229205766E-2</v>
+        <v>3.2516662395352641E-2</v>
       </c>
       <c r="E10" s="7">
-        <v>0.10522998470586059</v>
+        <v>0.19780127335509068</v>
       </c>
       <c r="F10" s="7">
-        <v>1.2928189565465003E-2</v>
+        <v>1.9392284348197522E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="3">
-        <v>2.1333333333333333E-2</v>
+        <v>6.7666666666666667E-2</v>
       </c>
       <c r="D11" s="3">
-        <v>1.0969655114602893E-2</v>
+        <v>2.1939310229205766E-2</v>
       </c>
       <c r="E11" s="7">
-        <v>4.5929807167730007E-2</v>
+        <v>0.10522998470586059</v>
       </c>
       <c r="F11" s="7">
-        <v>6.4640947827326409E-3</v>
+        <v>1.2928189565465003E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12" s="3">
-        <v>4.6333333333333337E-2</v>
+        <v>2.1333333333333333E-2</v>
       </c>
       <c r="D12" s="3">
-        <v>1.0969655114602853E-2</v>
+        <v>1.0969655114602893E-2</v>
       </c>
       <c r="E12" s="7">
-        <v>5.9300177538130029E-2</v>
+        <v>4.5929807167730007E-2</v>
       </c>
       <c r="F12" s="7">
-        <v>6.4640947827325299E-3</v>
+        <v>6.4640947827326409E-3</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C13" s="3">
         <v>4.6333333333333337E-2</v>
       </c>
@@ -815,15 +823,15 @@
         <v>1.0969655114602853E-2</v>
       </c>
       <c r="E13" s="7">
-        <v>5.9300177538130334E-2</v>
+        <v>5.9300177538130029E-2</v>
       </c>
       <c r="F13" s="7">
-        <v>6.4640947827325594E-3</v>
+        <v>6.4640947827325299E-3</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3">
@@ -833,249 +841,287 @@
         <v>1.0969655114602853E-2</v>
       </c>
       <c r="E14" s="7">
-        <v>5.9300177538130029E-2</v>
+        <v>5.9300177538130334E-2</v>
       </c>
       <c r="F14" s="7">
-        <v>6.4640947827326236E-3</v>
+        <v>6.4640947827325594E-3</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="3">
-        <v>0.59233333333333327</v>
+        <v>4.6333333333333337E-2</v>
       </c>
       <c r="D15" s="3">
-        <v>8.5049005481153891E-3</v>
+        <v>1.0969655114602853E-2</v>
       </c>
       <c r="E15" s="7">
-        <v>0.71133959924926959</v>
+        <v>5.9300177538130029E-2</v>
       </c>
       <c r="F15" s="7">
-        <v>6.8510243940337803E-3</v>
+        <v>6.4640947827326236E-3</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" s="3">
-        <v>0.45766666666666667</v>
+        <v>0.59233333333333327</v>
       </c>
       <c r="D16" s="3">
-        <v>1.3650396819628834E-2</v>
+        <v>8.5049005481153891E-3</v>
       </c>
       <c r="E16" s="7">
-        <v>0.66577647118717265</v>
+        <v>0.71133959924926959</v>
       </c>
       <c r="F16" s="7">
-        <v>1.654753817591019E-2</v>
+        <v>6.8510243940337803E-3</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3">
-        <v>1.2626666666666666</v>
+        <v>0.45766666666666667</v>
       </c>
       <c r="D17" s="3">
-        <v>1.0969655114602855E-2</v>
+        <v>1.3650396819628834E-2</v>
       </c>
       <c r="E17" s="7">
-        <v>1.4111429302193201</v>
+        <v>0.66577647118717265</v>
       </c>
       <c r="F17" s="7">
-        <v>1.5461980140142766E-2</v>
+        <v>1.654753817591019E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="C18" s="3">
-        <v>0.71499999999999986</v>
+        <v>0.45766666666666667</v>
       </c>
       <c r="D18" s="3">
-        <v>2.5632011235952615E-2</v>
+        <v>1.3650396819628834E-2</v>
       </c>
       <c r="E18" s="7">
-        <v>8.8320720625593804E-2</v>
+        <v>0.66577647118717265</v>
       </c>
       <c r="F18" s="7">
-        <v>6.4799155581467338E-3</v>
+        <v>1.654753817591019E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C19" s="3">
-        <v>0.65333333333333332</v>
+        <v>1.2626666666666666</v>
       </c>
       <c r="D19" s="3">
-        <v>8.0829037686547672E-3</v>
+        <v>1.0969655114602855E-2</v>
       </c>
       <c r="E19" s="7">
-        <v>1.0331686118053881E-2</v>
+        <v>1.4111429302193201</v>
       </c>
       <c r="F19" s="7">
-        <v>4.7474564212208262E-3</v>
+        <v>1.5461980140142766E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C20" s="3">
-        <v>1.6059999999999999</v>
+        <v>0.71499999999999986</v>
       </c>
       <c r="D20" s="3">
-        <v>2.5632011235952566E-2</v>
+        <v>2.5632011235952615E-2</v>
       </c>
       <c r="E20" s="7">
-        <v>1.0266847946996434</v>
+        <v>8.8320720625593804E-2</v>
       </c>
       <c r="F20" s="7">
-        <v>6.479915558148969E-3</v>
+        <v>6.4799155581467338E-3</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C21" s="3">
-        <v>0.26</v>
+        <v>0.65333333333333332</v>
       </c>
       <c r="D21" s="3">
-        <v>1.252996408614168E-2</v>
+        <v>8.0829037686547672E-3</v>
       </c>
       <c r="E21" s="7">
-        <v>0.11170565856824566</v>
+        <v>1.0331686118053881E-2</v>
       </c>
       <c r="F21" s="7">
-        <v>9.7156936859550819E-3</v>
+        <v>4.7474564212208262E-3</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="C22" s="3">
-        <v>6.6000000000000003E-2</v>
+        <v>1.6059999999999999</v>
       </c>
       <c r="D22" s="3">
-        <v>8.1853527718723576E-3</v>
+        <v>2.5632011235952566E-2</v>
       </c>
       <c r="E22" s="7">
-        <v>5.6093622719458102E-3</v>
+        <v>1.0266847946996434</v>
       </c>
       <c r="F22" s="7">
-        <v>9.7156936859549674E-3</v>
+        <v>6.479915558148969E-3</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="C23" s="3">
-        <v>6.6000000000000003E-2</v>
+        <v>0.26</v>
       </c>
       <c r="D23" s="3">
-        <v>8.1853527718723576E-3</v>
+        <v>1.252996408614168E-2</v>
       </c>
       <c r="E23" s="7">
-        <v>5.6093622719458102E-3</v>
+        <v>0.11170565856824566</v>
       </c>
       <c r="F23" s="7">
-        <v>9.7156936859549674E-3</v>
+        <v>9.7156936859550819E-3</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C24" s="3">
-        <v>0.48100000000000004</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="D24" s="3">
-        <v>1.0000000000000009E-3</v>
+        <v>8.1853527718723576E-3</v>
       </c>
       <c r="E24" s="7">
-        <v>0.53128084429100964</v>
+        <v>5.6093622719458102E-3</v>
       </c>
       <c r="F24" s="7">
-        <v>1.9386155643968311E-2</v>
+        <v>9.7156936859549674E-3</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="3">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D25" s="3">
+        <v>8.1853527718723576E-3</v>
+      </c>
+      <c r="E25" s="7">
+        <v>5.6093622719458102E-3</v>
+      </c>
+      <c r="F25" s="7">
+        <v>9.7156936859549674E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.48100000000000004</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1.0000000000000009E-3</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0.53128084429100964</v>
+      </c>
+      <c r="F26" s="7">
+        <v>1.9386155643968311E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2.0808652046684892E-2</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.82686125089241591</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1.1014147986613198E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B28" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="3">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="D25" s="3">
-        <v>2.0808652046684892E-2</v>
-      </c>
-      <c r="E25" s="7">
-        <v>0.82686125089241591</v>
-      </c>
-      <c r="F25" s="7">
-        <v>1.1014147986613198E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="6">
+      <c r="C28" s="6">
         <v>0.33366666666666672</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D28" s="6">
         <v>8.0829037686547672E-3</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E28" s="8">
         <v>5.7097170164858756E-3</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F28" s="8">
         <v>5.2865226367448141E-3</v>
       </c>
     </row>

</xml_diff>